<commit_message>
Added comments; removed distrustful validation code.
</commit_message>
<xml_diff>
--- a/tests/sample_files/entity_dictionaries/foo__mapping.xlsx
+++ b/tests/sample_files/entity_dictionaries/foo__mapping.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="5850" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="6300" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Entities" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
   <si>
     <t>authority</t>
   </si>
@@ -58,34 +58,13 @@
   </si>
   <si>
     <t>Lorem ...</t>
-  </si>
-  <si>
-    <t>bar {abc}Bar</t>
-  </si>
-  <si>
-    <t>asd</t>
-  </si>
-  <si>
-    <t>dfg</t>
-  </si>
-  <si>
-    <t>bar{abc} Bar</t>
-  </si>
-  <si>
-    <t>{123}</t>
-  </si>
-  <si>
-    <t>{123} {abc}</t>
-  </si>
-  <si>
-    <t>foo {abc} bar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -95,6 +74,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -122,9 +108,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -405,19 +392,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -438,139 +426,54 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" t="b">
+      <c r="C2" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C3" t="b">
+      <c r="C3" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C4" t="b">
+      <c r="C4" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="2" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" t="b">
-        <v>0</v>
-      </c>
-      <c r="D7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" t="b">
-        <v>0</v>
-      </c>
-      <c r="D8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>